<commit_message>
EPICP-1 DDs for Tracy and Ines
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
@@ -1,22 +1,201 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{314078C7-39FA-4351-9A3A-44458964D212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>valueType</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>BMI0</t>
+  </si>
+  <si>
+    <t>BMI at baseline</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>gj</t>
+  </si>
+  <si>
+    <t>corr_trigly</t>
+  </si>
+  <si>
+    <t>corr_chol</t>
+  </si>
+  <si>
+    <t>corr_hdl</t>
+  </si>
+  <si>
+    <t>bmi_f4</t>
+  </si>
+  <si>
+    <t>BMI at FUP4</t>
+  </si>
+  <si>
+    <t>waist</t>
+  </si>
+  <si>
+    <t>hip</t>
+  </si>
+  <si>
+    <t>waist_f4</t>
+  </si>
+  <si>
+    <t>hip_f4</t>
+  </si>
+  <si>
+    <t>age_anth_f4</t>
+  </si>
+  <si>
+    <t>zk</t>
+  </si>
+  <si>
+    <t>ze</t>
+  </si>
+  <si>
+    <t>zf</t>
+  </si>
+  <si>
+    <t>za</t>
+  </si>
+  <si>
+    <t>zb</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>fu</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>kd</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>kmt</t>
+  </si>
+  <si>
+    <t>kmf</t>
+  </si>
+  <si>
+    <t>mna</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>age of anthropometric measurement at FUP4</t>
+  </si>
+  <si>
+    <t>corrected triglycerides [mg/dL]</t>
+  </si>
+  <si>
+    <t>corrected cholesterol [mg/dL]</t>
+  </si>
+  <si>
+    <t>corrected HDL cholesterol [mg/dL]</t>
+  </si>
+  <si>
+    <t>glucose intakeat baseline [g/d]</t>
+  </si>
+  <si>
+    <t>fructose intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>carbohydrate intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>protein intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>fat intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>alcohol intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>fiber intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>saturated fatty acid intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>monounsaturated fatty acid intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>polyunsaturated fatty acid intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>disaccharide intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>monosaccharide intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>Total energy intake at baseline [kJ/d]</t>
+  </si>
+  <si>
+    <t>hip circumference at FUP4 [cm]</t>
+  </si>
+  <si>
+    <t>waist circumference at baseline [cm]</t>
+  </si>
+  <si>
+    <t>hip circumference at baseline [cm]</t>
+  </si>
+  <si>
+    <t>waist circumference at FUP4 [cm]</t>
+  </si>
+  <si>
+    <t>natrium intake at baseline [mg/d]</t>
+  </si>
+  <si>
+    <t>potassium intake at baseline [mg/d]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,6 +207,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -53,22 +238,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -110,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +336,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +388,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,33 +581,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>valueType</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -386,28 +889,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPICP-1 changed unit from mg/d to g/d for sodium and potassium intake in DD_EPICP_INES
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{314078C7-39FA-4351-9A3A-44458964D212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{A913CE29-CB27-48EC-A6FE-2749DCACAAED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,10 +185,10 @@
     <t>waist circumference at FUP4 [cm]</t>
   </si>
   <si>
-    <t>natrium intake at baseline [mg/d]</t>
-  </si>
-  <si>
-    <t>potassium intake at baseline [mg/d]</t>
+    <t>potassium intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>sodium intake at baseline [g/d]</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -877,7 +877,7 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
EPICP-1 changed DPE and DD for Tracy and Ines with regards to variable names, changed DPE for Franzi to remove some leftovers in the variable column
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_EPICP_INES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{A913CE29-CB27-48EC-A6FE-2749DCACAAED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{19B45B09-B959-43EE-A1B2-DED24FEC49E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -38,18 +38,12 @@
     <t>variable</t>
   </si>
   <si>
-    <t>BMI0</t>
-  </si>
-  <si>
     <t>BMI at baseline</t>
   </si>
   <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>gj</t>
-  </si>
-  <si>
     <t>corr_trigly</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
     <t>BMI at FUP4</t>
   </si>
   <si>
-    <t>waist</t>
-  </si>
-  <si>
-    <t>hip</t>
-  </si>
-  <si>
     <t>waist_f4</t>
   </si>
   <si>
@@ -80,48 +68,6 @@
     <t>age_anth_f4</t>
   </si>
   <si>
-    <t>zk</t>
-  </si>
-  <si>
-    <t>ze</t>
-  </si>
-  <si>
-    <t>zf</t>
-  </si>
-  <si>
-    <t>za</t>
-  </si>
-  <si>
-    <t>zb</t>
-  </si>
-  <si>
-    <t>fs</t>
-  </si>
-  <si>
-    <t>fu</t>
-  </si>
-  <si>
-    <t>fp</t>
-  </si>
-  <si>
-    <t>kd</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>kmt</t>
-  </si>
-  <si>
-    <t>kmf</t>
-  </si>
-  <si>
-    <t>mna</t>
-  </si>
-  <si>
-    <t>mk</t>
-  </si>
-  <si>
     <t>age of anthropometric measurement at FUP4</t>
   </si>
   <si>
@@ -189,6 +135,60 @@
   </si>
   <si>
     <t>sodium intake at baseline [g/d]</t>
+  </si>
+  <si>
+    <t>bmi0</t>
+  </si>
+  <si>
+    <t>GJ</t>
+  </si>
+  <si>
+    <t>waist0</t>
+  </si>
+  <si>
+    <t>hip0</t>
+  </si>
+  <si>
+    <t>ZK</t>
+  </si>
+  <si>
+    <t>ZE</t>
+  </si>
+  <si>
+    <t>ZF</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>ZB</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>KMT</t>
+  </si>
+  <si>
+    <t>KMF</t>
+  </si>
+  <si>
+    <t>MNA</t>
+  </si>
+  <si>
+    <t>MK</t>
   </si>
 </sst>
 </file>
@@ -584,17 +584,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,279 +608,279 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -894,9 +894,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>